<commit_message>
further development in axis control board
</commit_message>
<xml_diff>
--- a/Mechanics/water_distribution_BOM.xlsx
+++ b/Mechanics/water_distribution_BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambadran717/Projects/SIMACAS/Electronics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambadran717/Desktop/tmp_simacas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72EB50B-05CF-0A47-AB4C-B5D02E56FA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E2AF22-87CA-6946-AB93-03A8489266FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{4BDA6589-EB7D-AB42-8496-E99172E28F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>No.</t>
   </si>
@@ -59,55 +59,52 @@
     <t>Store</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>UGE</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>DC pump</t>
-  </si>
-  <si>
     <t>solenoid valve</t>
   </si>
   <si>
-    <t>Relay Module 12V 4Channel</t>
-  </si>
-  <si>
-    <t>Water hose</t>
-  </si>
-  <si>
-    <t>6mm internal diameter 8mm external diameter</t>
-  </si>
-  <si>
-    <t>fittings</t>
-  </si>
-  <si>
-    <t>Hose splitter 1 to 6</t>
-  </si>
-  <si>
-    <t>3D printed</t>
-  </si>
-  <si>
-    <t>PWM Power Control board</t>
-  </si>
-  <si>
-    <t>irfz44n based PCB with opto-coupler insulation</t>
-  </si>
-  <si>
-    <t>Power Supply 12V 10Amps</t>
-  </si>
-  <si>
-    <t>3D printed water demultiplexer from 1 pump to 6 valves</t>
-  </si>
-  <si>
     <t>circuits electronics</t>
   </si>
   <si>
-    <t>HD electronics</t>
+    <t>Power wires 1.5mm</t>
+  </si>
+  <si>
+    <t>From 1/2 inch diameter hose to 3/4 inch inlet of solenoid valve</t>
+  </si>
+  <si>
+    <t>2 from 2 different sources to distributer, 6 from distributer to 3 axis of 2 different sprinkler each</t>
+  </si>
+  <si>
+    <t>large female spade/ crimp</t>
+  </si>
+  <si>
+    <t>for input of solenoid valve</t>
+  </si>
+  <si>
+    <t>Hose tightenner</t>
+  </si>
+  <si>
+    <t>Fitting 3/4inch female to 1/2inch hose</t>
+  </si>
+  <si>
+    <t>for solenoids and relays</t>
+  </si>
+  <si>
+    <t>Water distributer 1 to 3</t>
+  </si>
+  <si>
+    <t>3D printed water distributer from 1 source to 6 outputs</t>
+  </si>
+  <si>
+    <t>Power supply 12v 10Amps</t>
+  </si>
+  <si>
+    <t>Relay Module 12V 3Channel</t>
+  </si>
+  <si>
+    <t>hose 1/2 inch diameter</t>
   </si>
 </sst>
 </file>
@@ -139,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -163,81 +160,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -375,119 +307,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -539,6 +358,88 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -554,45 +455,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,257 +827,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FB5A49-5513-9042-874B-8A1BAD4D0C64}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1400</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5">
-        <f>C2*D2</f>
-        <v>1400</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="6" t="s">
+      <c r="B2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="C2" s="22">
+        <v>15</v>
+      </c>
+      <c r="D2" s="22">
+        <v>30</v>
+      </c>
+      <c r="E2" s="23">
+        <f t="shared" ref="E2:E3" si="0">C2*D2</f>
+        <v>450</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="11">
-        <f t="shared" ref="E3:E9" si="0">C3*D3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="27" t="s">
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3">
         <v>20</v>
       </c>
-      <c r="C4" s="8">
-        <v>375</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11">
-        <f t="shared" si="0"/>
-        <v>375</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8">
-        <v>250</v>
-      </c>
-      <c r="D6" s="8">
-        <v>6</v>
-      </c>
-      <c r="E6" s="11">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="27" t="s">
+      <c r="D3" s="3">
         <v>12</v>
       </c>
-      <c r="C7" s="8">
-        <v>150</v>
-      </c>
-      <c r="D7" s="8">
-        <v>2</v>
-      </c>
-      <c r="E7" s="11">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="8">
-        <v>30</v>
-      </c>
-      <c r="D8" s="8">
-        <v>8</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="E3" s="6">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>250</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" ref="E4:E10" si="1">C4*D4</f>
+        <v>1500</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>375</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <v>120</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>200</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="1">
         <f>SUM(E2:E11)</f>
-        <v>3815</v>
-      </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="16"/>
+        <v>3279</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>